<commit_message>
Updated Undecomposed Model to include Heat store - 02/12/23
</commit_message>
<xml_diff>
--- a/Greenfield Model copy/OREIA3_2017/data/algorithm.xlsx
+++ b/Greenfield Model copy/OREIA3_2017/data/algorithm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel/Desktop/Edinburgh MMath Degree Stuff/MMath Diss/Greenfield Model copy/OREIA3_2017/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/axel/Desktop/Edinburgh MMath Degree Stuff/MMath Diss/Year5-MMath-Diss/Greenfield Model copy/OREIA3_2017/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A9293F-C82A-C04E-B8CC-B3740138810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7577DD8D-0677-FF4B-BA0F-4F282ACC3F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3380" yWindow="3380" windowWidth="21600" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="parameters" sheetId="3" r:id="rId3"/>
     <sheet name="readme" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 

</xml_diff>